<commit_message>
Updated Schematic to v1.0.1
made chante to Vref Capacitors. Was 3.3uF, now 22uF
</commit_message>
<xml_diff>
--- a/Ganglion_01_BOM.xlsx
+++ b/Ganglion_01_BOM.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="985" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="199">
   <si>
     <t>Item</t>
   </si>
@@ -41,9 +41,6 @@
     <t>QTY</t>
   </si>
   <si>
-    <t>Consigned by OpenBCI</t>
-  </si>
-  <si>
     <t>B1</t>
   </si>
   <si>
@@ -131,13 +128,10 @@
     <t>C9,C37,C39,C44</t>
   </si>
   <si>
-    <t>3.3uF</t>
-  </si>
-  <si>
-    <t>C0603C335M9PACTU</t>
-  </si>
-  <si>
-    <t>Kemet</t>
+    <t>22uF</t>
+  </si>
+  <si>
+    <t>GRM188R60J226MEA0D</t>
   </si>
   <si>
     <t>D1</t>
@@ -414,9 +408,6 @@
   </si>
   <si>
     <t>OpenBCI:ST-TF-0003A</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>U14</t>
@@ -636,6 +627,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -657,22 +649,57 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -701,7 +728,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -710,20 +737,28 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -745,8 +780,8 @@
   </sheetPr>
   <dimension ref="A1:J42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -756,12 +791,12 @@
     <col collapsed="false" hidden="false" max="4" min="3" style="0" width="11.5204081632653"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.6734693877551"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="19.5816326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="19.5816326530612"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -782,1182 +817,1176 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="5"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="2"/>
+      <c r="H2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+      <c r="A3" s="2" t="n">
         <f aca="false">A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="4" t="n">
         <v>15</v>
       </c>
       <c r="I3" s="5"/>
-      <c r="J3" s="2"/>
+      <c r="J3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+      <c r="A4" s="2" t="n">
         <f aca="false">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="F4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="4" t="n">
         <v>4</v>
       </c>
       <c r="I4" s="5"/>
-      <c r="J4" s="2"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+      <c r="A5" s="2" t="n">
         <f aca="false">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2"/>
+      <c r="H5" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+      <c r="A6" s="2" t="n">
         <f aca="false">A5+1</f>
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2"/>
+      <c r="H6" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+      <c r="A7" s="2" t="n">
         <f aca="false">A6+1</f>
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="F7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="J7" s="2"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+      <c r="A8" s="2" t="n">
         <f aca="false">A7+1</f>
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="F8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="4" t="n">
         <v>19</v>
       </c>
       <c r="I8" s="5"/>
-      <c r="J8" s="2"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+      <c r="A9" s="2" t="n">
         <f aca="false">A8+1</f>
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="F9" s="3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="H9" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J9" s="2"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+      <c r="A10" s="2" t="n">
         <f aca="false">A9+1</f>
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="E10" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="H10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="2" t="n">
         <f aca="false">A10+1</f>
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H11" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2"/>
+      <c r="H11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+      <c r="A12" s="2" t="n">
         <f aca="false">A11+1</f>
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H12" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J12" s="2"/>
+      <c r="H12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+      <c r="A13" s="2" t="n">
         <f aca="false">A12+1</f>
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="3" t="n">
+      <c r="H13" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="J13" s="2"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+      <c r="A14" s="2" t="n">
         <f aca="false">A13+1</f>
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="E14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="F14" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" s="3" t="n">
+      <c r="H14" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="2"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="n">
+      <c r="A15" s="2" t="n">
         <f aca="false">A14+1</f>
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="E15" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H15" s="3" t="n">
+      <c r="H15" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J15" s="2"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="n">
+      <c r="A16" s="2" t="n">
         <f aca="false">A15+1</f>
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="G16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H16" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="H16" s="4" t="n">
         <v>10</v>
       </c>
       <c r="I16" s="5"/>
-      <c r="J16" s="2"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="n">
+      <c r="A17" s="2" t="n">
         <f aca="false">A16+1</f>
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D17" s="3" t="s">
+      <c r="F17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H17" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="H17" s="4" t="n">
         <v>7</v>
       </c>
       <c r="I17" s="5"/>
-      <c r="J17" s="2"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="n">
+      <c r="A18" s="2" t="n">
         <f aca="false">A17+1</f>
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="F18" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="H18" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J18" s="2"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="n">
+      <c r="A19" s="2" t="n">
         <f aca="false">A18+1</f>
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="F19" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H19" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="H19" s="4" t="n">
         <v>12</v>
       </c>
-      <c r="J19" s="2"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="n">
+      <c r="A20" s="2" t="n">
         <f aca="false">A19+1</f>
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="F20" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H20" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="H20" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I20" s="5"/>
-      <c r="J20" s="2"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="n">
+      <c r="A21" s="2" t="n">
         <f aca="false">A20+1</f>
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>72</v>
+      <c r="F21" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J21" s="2"/>
+        <v>71</v>
+      </c>
+      <c r="H21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="n">
+      <c r="A22" s="2" t="n">
         <f aca="false">A21+1</f>
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>72</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="H22" s="3" t="n">
+        <v>71</v>
+      </c>
+      <c r="H22" s="4" t="n">
         <v>10</v>
       </c>
       <c r="I22" s="5"/>
-      <c r="J22" s="2"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="n">
+      <c r="A23" s="2" t="n">
         <f aca="false">A22+1</f>
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="E23" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="F23" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="H23" s="3" t="n">
+      <c r="H23" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J23" s="2"/>
+      <c r="J23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="n">
+      <c r="A24" s="2" t="n">
         <f aca="false">A23+1</f>
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="F24" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H24" s="3" t="n">
+      <c r="H24" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="2"/>
+      <c r="J24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="n">
+      <c r="A25" s="2" t="n">
         <f aca="false">A24+1</f>
         <v>24</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="3" t="s">
+      <c r="E25" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="F25" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H25" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J25" s="2"/>
+      <c r="H25" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="n">
+      <c r="A26" s="2" t="n">
         <f aca="false">A25+1</f>
         <v>25</v>
       </c>
       <c r="B26" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D26" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H26" s="3" t="n">
+      <c r="H26" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I26" s="5"/>
-      <c r="J26" s="2"/>
+      <c r="J26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="n">
+      <c r="A27" s="2" t="n">
         <f aca="false">A26+1</f>
         <v>26</v>
       </c>
       <c r="B27" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="E27" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="F27" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H27" s="3" t="n">
+      <c r="H27" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I27" s="5"/>
-      <c r="J27" s="2"/>
+      <c r="J27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
+      <c r="A28" s="2" t="n">
         <f aca="false">A27+1</f>
         <v>27</v>
       </c>
       <c r="B28" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="E28" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="F28" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G28" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H28" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="J28" s="2"/>
+      <c r="H28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
+      <c r="A29" s="2" t="n">
         <f aca="false">A28+1</f>
         <v>28</v>
       </c>
       <c r="B29" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="F29" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>138</v>
-      </c>
       <c r="G29" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H29" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="H29" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I29" s="5"/>
-      <c r="J29" s="2"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1" t="n">
+      <c r="A30" s="2" t="n">
         <f aca="false">A29+1</f>
         <v>29</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G30" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G30" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H30" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J30" s="2"/>
+      <c r="H30" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1" t="n">
+      <c r="A31" s="2" t="n">
         <f aca="false">A30+1</f>
         <v>30</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="G31" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H31" s="3" t="n">
+        <v>139</v>
+      </c>
+      <c r="H31" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I31" s="5"/>
-      <c r="J31" s="2"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1" t="n">
+      <c r="A32" s="2" t="n">
         <f aca="false">A31+1</f>
         <v>31</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="H32" s="3" t="n">
+      <c r="H32" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I32" s="5"/>
-      <c r="J32" s="2"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1" t="n">
+      <c r="A33" s="2" t="n">
         <f aca="false">A32+1</f>
         <v>32</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="F33" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="D33" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H33" s="3" t="n">
+      <c r="H33" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="J33" s="2"/>
+      <c r="J33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1" t="n">
+      <c r="A34" s="2" t="n">
         <f aca="false">A33+1</f>
         <v>33</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E34" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="F34" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="D34" s="4" t="s">
+      <c r="G34" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G34" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H34" s="3" t="n">
+      <c r="H34" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J34" s="2"/>
+      <c r="J34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <f aca="false">A34+1</f>
         <v>34</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="F35" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G35" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>167</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="H35" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J35" s="2"/>
+      <c r="H35" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="1" t="n">
+      <c r="A36" s="2" t="n">
         <f aca="false">A35+1</f>
         <v>35</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="H36" s="3" t="n">
+        <v>139</v>
+      </c>
+      <c r="H36" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="J36" s="2"/>
+      <c r="J36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="1" t="n">
+      <c r="A37" s="2" t="n">
         <f aca="false">A36+1</f>
         <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>176</v>
-      </c>
       <c r="F37" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="H37" s="3" t="n">
+        <v>124</v>
+      </c>
+      <c r="H37" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="J37" s="2"/>
+      <c r="J37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
+      <c r="A38" s="2" t="n">
         <f aca="false">A37+1</f>
         <v>37</v>
       </c>
       <c r="B38" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>138</v>
+      <c r="F38" s="6" t="s">
+        <v>135</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="H38" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J38" s="2"/>
+        <v>155</v>
+      </c>
+      <c r="H38" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="n">
+      <c r="A39" s="2" t="n">
         <f aca="false">A38+1</f>
         <v>38</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="F39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G39" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D39" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="H39" s="3" t="n">
+      <c r="H39" s="4" t="n">
         <v>1</v>
       </c>
       <c r="I39" s="5"/>
-      <c r="J39" s="2"/>
+      <c r="J39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="1" t="n">
+      <c r="A40" s="2" t="n">
         <f aca="false">A39+1</f>
         <v>39</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="F40" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="G40" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H40" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="I40" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="J40" s="2"/>
+      <c r="H40" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <f aca="false">A40+1</f>
         <v>40</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>119</v>
+      <c r="F41" s="6" t="s">
+        <v>117</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="H41" s="3" t="n">
+        <v>118</v>
+      </c>
+      <c r="H41" s="4" t="n">
         <v>2</v>
       </c>
       <c r="I41" s="5"/>
-      <c r="J41" s="2"/>
+      <c r="J41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="n">
+      <c r="A42" s="2" t="n">
         <f aca="false">A41+1</f>
         <v>41</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="F42" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="H42" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="J42" s="2"/>
+      <c r="H42" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="J42" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>